<commit_message>
2:34 - 24 - Jan
</commit_message>
<xml_diff>
--- a/testing_2/00_Others/State_of_fsm_V2.xlsx
+++ b/testing_2/00_Others/State_of_fsm_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TAI_LIEU\ET-E9\Program\20231\Microprocessor\Lab_work\lab05_trafic_light\00_Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TAI_LIEU\ET-E9\Program\20231\Microprocessor\Lab_work\testing_2\00_Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4985EC86-CA03-43CE-9646-9F550FFBDE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9347DB41-E411-4BAF-8050-442A04B23201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90F95703-22D4-423E-B6F2-5ECC34AEAC1F}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,23 +424,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,15 +461,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>398178</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>153839</xdr:rowOff>
+      <xdr:colOff>17178</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>58589</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
+      <xdr:colOff>95251</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>80413</xdr:rowOff>
+      <xdr:rowOff>175663</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -495,8 +492,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3552358" y="2589741"/>
-          <a:ext cx="5558852" cy="1612967"/>
+          <a:off x="3169953" y="2725589"/>
+          <a:ext cx="5564473" cy="1641074"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -807,9 +804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199C2C26-4FE3-48F8-B1B6-412F5898A14E}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y14" sqref="Y14"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,55 +817,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="10" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
@@ -896,22 +893,22 @@
       <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
@@ -939,30 +936,30 @@
       <c r="M3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="12" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1009,7 +1006,7 @@
       <c r="N4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="4">
         <v>10</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -1080,31 +1077,31 @@
       <c r="N5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="4">
         <v>2</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="U5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="V5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="W5" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1151,31 +1148,31 @@
       <c r="N6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="4">
         <v>1</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="S6" s="9" t="s">
         <v>44</v>
       </c>
       <c r="T6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="12" t="s">
+      <c r="U6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="12" t="s">
+      <c r="V6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="W6" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1222,7 +1219,7 @@
       <c r="N7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="4">
         <v>10</v>
       </c>
       <c r="P7" s="4" t="s">
@@ -1293,31 +1290,31 @@
       <c r="N8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="4">
         <v>2</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" s="9" t="s">
         <v>47</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="S8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="T8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="U8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="V8" s="12" t="s">
+      <c r="V8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="W8" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1364,31 +1361,31 @@
       <c r="N9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="4">
         <v>1</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="Q9" s="9" t="s">
         <v>45</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S9" s="12" t="s">
+      <c r="S9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="U9" s="12" t="s">
+      <c r="U9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="V9" s="12" t="s">
+      <c r="V9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="W9" s="12" t="s">
+      <c r="W9" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1435,7 +1432,7 @@
       <c r="N10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="4">
         <v>8</v>
       </c>
       <c r="P10" s="4" t="s">
@@ -1506,7 +1503,7 @@
       <c r="N11" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="4">
         <v>2</v>
       </c>
       <c r="P11" s="4" t="s">
@@ -1515,22 +1512,22 @@
       <c r="Q11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="12" t="s">
+      <c r="R11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="S11" s="12" t="s">
+      <c r="S11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="T11" s="12" t="s">
+      <c r="T11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="U11" s="12" t="s">
+      <c r="U11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="V11" s="12" t="s">
+      <c r="V11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="W11" s="12" t="s">
+      <c r="W11" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1577,7 +1574,7 @@
       <c r="N12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="4">
         <v>1</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -1586,22 +1583,22 @@
       <c r="Q12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R12" s="12" t="s">
+      <c r="R12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="12" t="s">
+      <c r="S12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="T12" s="12" t="s">
+      <c r="T12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="U12" s="12" t="s">
+      <c r="U12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="V12" s="12" t="s">
+      <c r="V12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="W12" s="12" t="s">
+      <c r="W12" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1648,31 +1645,31 @@
       <c r="N13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="4">
         <v>2</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q13" s="12" t="s">
+      <c r="Q13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="R13" s="12" t="s">
+      <c r="R13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="S13" s="12" t="s">
+      <c r="S13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="T13" s="12" t="s">
+      <c r="T13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="U13" s="12" t="s">
+      <c r="U13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="V13" s="12" t="s">
+      <c r="V13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="W13" s="12" t="s">
+      <c r="W13" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1690,7 +1687,7 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="10" t="s">
         <v>77</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1705,7 +1702,7 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="10" t="s">
         <v>64</v>
       </c>
       <c r="D17" s="2">
@@ -1720,7 +1717,7 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D18" s="1">
@@ -1738,7 +1735,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D19"/>
@@ -1751,7 +1748,7 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D20"/>
@@ -1764,7 +1761,7 @@
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D21"/>
@@ -1780,17 +1777,17 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="10" t="s">
         <v>71</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1798,27 +1795,27 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="10" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>